<commit_message>
fixed a bug in the quartiles for data
</commit_message>
<xml_diff>
--- a/DOF/E-6_Report_July_2010-2019_w.xlsx
+++ b/DOF/E-6_Report_July_2010-2019_w.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/aaronm6_illinois_edu/Documents/School/cs416-su25/dashboard project/DOF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{B42FECB8-6F88-424C-AD59-3088CC1E374C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F20A01DF-F2CA-412F-ABD4-715528E8987C}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{B42FECB8-6F88-424C-AD59-3088CC1E374C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B55478BC-B79B-4E71-AF90-16BEDEC7AC44}"/>
   <bookViews>
     <workbookView xWindow="-21900" yWindow="-21720" windowWidth="21840" windowHeight="37920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="96">
   <si>
     <t>Births</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Colusa</t>
-  </si>
-  <si>
-    <t>Costa</t>
   </si>
   <si>
     <t>Del Norte</t>
@@ -228,9 +225,6 @@
     <t>Yuba</t>
   </si>
   <si>
-    <t xml:space="preserve">Contra </t>
-  </si>
-  <si>
     <t>San</t>
   </si>
   <si>
@@ -340,6 +334,9 @@
   </si>
   <si>
     <t>State of California, Department of Finance, E-6. Population Estimates and Components of Change by County — July 1, 2010–2019, December 2021</t>
+  </si>
+  <si>
+    <t>Contra Costa</t>
   </si>
 </sst>
 </file>
@@ -1027,69 +1024,69 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,8 +1107,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K726"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N76" sqref="N76:N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1133,48 +1130,48 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="69"/>
       <c r="J2" s="70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K2" s="71" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>85</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="71" t="s">
         <v>86</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="71" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24"/>
       <c r="B4" s="25"/>
       <c r="C4" s="72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>0</v>
@@ -1183,16 +1180,16 @@
         <v>1</v>
       </c>
       <c r="H4" s="73" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" s="74" t="s">
-        <v>93</v>
-      </c>
       <c r="K4" s="75" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
@@ -1211,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="27">
         <v>37253956</v>
@@ -1230,7 +1227,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="8">
         <v>37363368</v>
@@ -1593,7 +1590,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="27">
         <v>1510271</v>
@@ -1612,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="27">
         <v>1516617</v>
@@ -1975,7 +1972,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30" s="27">
         <v>1175</v>
@@ -1994,7 +1991,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31" s="27">
         <v>1177</v>
@@ -2357,7 +2354,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" s="27">
         <v>38091</v>
@@ -2376,7 +2373,7 @@
         <v>5</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C43" s="27">
         <v>37714</v>
@@ -2739,7 +2736,7 @@
         <v>6</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C54" s="27">
         <v>220000</v>
@@ -2758,7 +2755,7 @@
         <v>6</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C55" s="27">
         <v>220619</v>
@@ -3121,7 +3118,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C66" s="27">
         <v>45578</v>
@@ -3140,7 +3137,7 @@
         <v>7</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C67" s="27">
         <v>45565</v>
@@ -3503,7 +3500,7 @@
         <v>8</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C78" s="27">
         <v>21419</v>
@@ -3522,7 +3519,7 @@
         <v>8</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C79" s="27">
         <v>21322</v>
@@ -3882,10 +3879,10 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="22" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B90" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C90" s="27">
         <v>1049025</v>
@@ -3901,10 +3898,10 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="22" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C91" s="27">
         <v>1053028</v>
@@ -3935,6 +3932,9 @@
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B92" s="29">
         <v>2011</v>
       </c>
@@ -3967,7 +3967,9 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="45"/>
+      <c r="A93" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B93" s="19">
         <v>2012</v>
       </c>
@@ -4000,7 +4002,9 @@
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="45"/>
+      <c r="A94" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B94" s="19">
         <v>2013</v>
       </c>
@@ -4033,7 +4037,9 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="45"/>
+      <c r="A95" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B95" s="19">
         <v>2014</v>
       </c>
@@ -4066,7 +4072,9 @@
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="45"/>
+      <c r="A96" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B96" s="19">
         <v>2015</v>
       </c>
@@ -4099,7 +4107,9 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="45"/>
+      <c r="A97" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B97" s="19">
         <v>2016</v>
       </c>
@@ -4132,7 +4142,9 @@
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="45"/>
+      <c r="A98" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B98" s="19">
         <v>2017</v>
       </c>
@@ -4165,7 +4177,9 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="45"/>
+      <c r="A99" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B99" s="19">
         <v>2018</v>
       </c>
@@ -4198,7 +4212,9 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="45"/>
+      <c r="A100" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="B100" s="19">
         <v>2019</v>
       </c>
@@ -4245,10 +4261,10 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C102" s="27">
         <v>28610</v>
@@ -4263,9 +4279,11 @@
       <c r="K102" s="27"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="49"/>
+      <c r="A103" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B103" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C103" s="27">
         <v>28421</v>
@@ -4296,7 +4314,9 @@
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="49"/>
+      <c r="A104" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B104" s="29">
         <v>2011</v>
       </c>
@@ -4329,7 +4349,9 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="49"/>
+      <c r="A105" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B105" s="19">
         <v>2012</v>
       </c>
@@ -4362,7 +4384,9 @@
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="49"/>
+      <c r="A106" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B106" s="19">
         <v>2013</v>
       </c>
@@ -4395,7 +4419,9 @@
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="49"/>
+      <c r="A107" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B107" s="19">
         <v>2014</v>
       </c>
@@ -4428,7 +4454,9 @@
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="49"/>
+      <c r="A108" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B108" s="19">
         <v>2015</v>
       </c>
@@ -4461,7 +4489,9 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="49"/>
+      <c r="A109" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B109" s="19">
         <v>2016</v>
       </c>
@@ -4494,7 +4524,9 @@
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="49"/>
+      <c r="A110" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B110" s="19">
         <v>2017</v>
       </c>
@@ -4527,7 +4559,9 @@
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="49"/>
+      <c r="A111" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B111" s="19">
         <v>2018</v>
       </c>
@@ -4560,7 +4594,9 @@
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="49"/>
+      <c r="A112" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="B112" s="19">
         <v>2019</v>
       </c>
@@ -4607,10 +4643,10 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B114" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C114" s="27">
         <v>181058</v>
@@ -4626,7 +4662,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B115" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C115" s="27">
         <v>181135</v>
@@ -4967,10 +5003,10 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C126" s="27">
         <v>930450</v>
@@ -4986,7 +5022,7 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B127" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C127" s="27">
         <v>932842</v>
@@ -5327,10 +5363,10 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B138" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C138" s="27">
         <v>28122</v>
@@ -5346,7 +5382,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B139" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C139" s="27">
         <v>28220</v>
@@ -5687,10 +5723,10 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B150" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C150" s="27">
         <v>134623</v>
@@ -5706,7 +5742,7 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B151" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C151" s="27">
         <v>135187</v>
@@ -6047,10 +6083,10 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B162" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C162" s="27">
         <v>174528</v>
@@ -6066,7 +6102,7 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B163" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C163" s="27">
         <v>175188</v>
@@ -6407,10 +6443,10 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B174" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C174" s="27">
         <v>18546</v>
@@ -6426,7 +6462,7 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B175" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C175" s="27">
         <v>18560</v>
@@ -6767,10 +6803,10 @@
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B186" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C186" s="27">
         <v>839631</v>
@@ -6786,7 +6822,7 @@
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B187" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C187" s="27">
         <v>841932</v>
@@ -7127,10 +7163,10 @@
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B198" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C198" s="27">
         <v>152982</v>
@@ -7146,7 +7182,7 @@
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B199" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C199" s="27">
         <v>152355</v>
@@ -7487,10 +7523,10 @@
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B210" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C210" s="27">
         <v>64665</v>
@@ -7506,7 +7542,7 @@
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B211" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C211" s="27">
         <v>65981</v>
@@ -7847,10 +7883,10 @@
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B222" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C222" s="27">
         <v>34895</v>
@@ -7866,7 +7902,7 @@
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B223" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C223" s="27">
         <v>34878</v>
@@ -8207,10 +8243,10 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B234" s="79" t="s">
         <v>66</v>
-      </c>
-      <c r="B234" s="79" t="s">
-        <v>68</v>
       </c>
       <c r="C234" s="57">
         <v>9818605</v>
@@ -8226,10 +8262,10 @@
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B235" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C235" s="27">
         <v>9842625</v>
@@ -8570,10 +8606,10 @@
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B246" s="56" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C246" s="57">
         <v>150865</v>
@@ -8589,7 +8625,7 @@
     </row>
     <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B247" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C247" s="27">
         <v>150123</v>
@@ -8930,10 +8966,10 @@
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C258" s="27">
         <v>252409</v>
@@ -8949,7 +8985,7 @@
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B259" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C259" s="27">
         <v>252750</v>
@@ -9290,10 +9326,10 @@
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B270" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C270" s="27">
         <v>18251</v>
@@ -9309,7 +9345,7 @@
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B271" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C271" s="27">
         <v>18228</v>
@@ -9650,10 +9686,10 @@
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B282" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C282" s="27">
         <v>87841</v>
@@ -9669,7 +9705,7 @@
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B283" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C283" s="27">
         <v>87856</v>
@@ -10010,10 +10046,10 @@
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B294" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C294" s="27">
         <v>255793</v>
@@ -10029,7 +10065,7 @@
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B295" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C295" s="27">
         <v>256705</v>
@@ -10370,10 +10406,10 @@
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B306" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C306" s="27">
         <v>9686</v>
@@ -10389,7 +10425,7 @@
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B307" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C307" s="27">
         <v>9713</v>
@@ -10730,10 +10766,10 @@
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B318" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C318" s="27">
         <v>14202</v>
@@ -10749,7 +10785,7 @@
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B319" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C319" s="27">
         <v>14011</v>
@@ -11090,10 +11126,10 @@
     </row>
     <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B330" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C330" s="27">
         <v>415057</v>
@@ -11109,7 +11145,7 @@
     </row>
     <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B331" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C331" s="27">
         <v>415956</v>
@@ -11450,10 +11486,10 @@
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B342" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C342" s="27">
         <v>136484</v>
@@ -11470,7 +11506,7 @@
     <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="49"/>
       <c r="B343" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C343" s="27">
         <v>136568</v>
@@ -11812,10 +11848,10 @@
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B354" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C354" s="27">
         <v>98764</v>
@@ -11831,7 +11867,7 @@
     </row>
     <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B355" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C355" s="27">
         <v>98834</v>
@@ -12172,10 +12208,10 @@
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B366" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C366" s="27">
         <v>3010232</v>
@@ -12191,7 +12227,7 @@
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B367" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C367" s="27">
         <v>3016922</v>
@@ -12532,10 +12568,10 @@
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B378" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C378" s="27">
         <v>348432</v>
@@ -12551,7 +12587,7 @@
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B379" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C379" s="27">
         <v>350872</v>
@@ -12892,10 +12928,10 @@
     </row>
     <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B390" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C390" s="27">
         <v>20007</v>
@@ -12911,7 +12947,7 @@
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B391" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C391" s="27">
         <v>19985</v>
@@ -13252,10 +13288,10 @@
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A402" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B402" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C402" s="27">
         <v>2189641</v>
@@ -13272,7 +13308,7 @@
     <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A403" s="49"/>
       <c r="B403" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C403" s="27">
         <v>2197839</v>
@@ -13614,10 +13650,10 @@
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B414" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C414" s="27">
         <v>1418788</v>
@@ -13633,7 +13669,7 @@
     </row>
     <row r="415" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B415" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C415" s="27">
         <v>1423634</v>
@@ -13974,10 +14010,10 @@
     </row>
     <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B426" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C426" s="27">
         <v>55269</v>
@@ -13993,7 +14029,7 @@
     </row>
     <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B427" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C427" s="27">
         <v>55563</v>
@@ -14334,10 +14370,10 @@
     </row>
     <row r="438" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A438" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B438" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C438" s="27">
         <v>2035210</v>
@@ -14353,10 +14389,10 @@
     </row>
     <row r="439" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A439" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B439" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C439" s="27">
         <v>2044954</v>
@@ -14697,10 +14733,10 @@
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B450" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C450" s="27">
         <v>3095313</v>
@@ -14716,7 +14752,7 @@
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B451" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C451" s="27">
         <v>3103511</v>
@@ -15057,10 +15093,10 @@
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A462" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B462" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C462" s="27">
         <v>805235</v>
@@ -15076,10 +15112,10 @@
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A463" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B463" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C463" s="27">
         <v>809945</v>
@@ -15421,10 +15457,10 @@
     </row>
     <row r="474" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A474" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B474" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C474" s="27">
         <v>685306</v>
@@ -15440,10 +15476,10 @@
     </row>
     <row r="475" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A475" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B475" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C475" s="27">
         <v>688585</v>
@@ -15784,10 +15820,10 @@
     </row>
     <row r="486" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A486" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B486" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C486" s="27">
         <v>269637</v>
@@ -15803,10 +15839,10 @@
     </row>
     <row r="487" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A487" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B487" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C487" s="27">
         <v>269604</v>
@@ -16147,10 +16183,10 @@
     </row>
     <row r="498" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A498" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B498" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C498" s="27">
         <v>718451</v>
@@ -16166,7 +16202,7 @@
     </row>
     <row r="499" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B499" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C499" s="27">
         <v>721169</v>
@@ -16519,10 +16555,10 @@
     </row>
     <row r="511" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A511" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B511" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C511" s="27">
         <v>423895</v>
@@ -16538,10 +16574,10 @@
     </row>
     <row r="512" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A512" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B512" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C512" s="27">
         <v>424045</v>
@@ -16882,10 +16918,10 @@
     </row>
     <row r="523" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A523" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B523" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C523" s="27">
         <v>1781642</v>
@@ -16901,10 +16937,10 @@
     </row>
     <row r="524" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A524" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B524" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C524" s="27">
         <v>1790845</v>
@@ -17245,10 +17281,10 @@
     </row>
     <row r="535" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A535" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B535" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C535" s="27">
         <v>262382</v>
@@ -17265,7 +17301,7 @@
     <row r="536" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A536" s="49"/>
       <c r="B536" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C536" s="27">
         <v>262828</v>
@@ -17607,10 +17643,10 @@
     </row>
     <row r="547" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A547" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B547" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C547" s="27">
         <v>177223</v>
@@ -17626,7 +17662,7 @@
     </row>
     <row r="548" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B548" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C548" s="27">
         <v>177488</v>
@@ -17967,10 +18003,10 @@
     </row>
     <row r="559" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A559" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B559" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C559" s="27">
         <v>3240</v>
@@ -17986,7 +18022,7 @@
     </row>
     <row r="560" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B560" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C560" s="27">
         <v>3236</v>
@@ -18327,10 +18363,10 @@
     </row>
     <row r="571" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A571" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B571" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C571" s="27">
         <v>44900</v>
@@ -18346,7 +18382,7 @@
     </row>
     <row r="572" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B572" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C572" s="27">
         <v>44859</v>
@@ -18687,10 +18723,10 @@
     </row>
     <row r="583" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A583" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B583" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C583" s="27">
         <v>413344</v>
@@ -18706,7 +18742,7 @@
     </row>
     <row r="584" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B584" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C584" s="27">
         <v>413197</v>
@@ -19047,10 +19083,10 @@
     </row>
     <row r="595" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A595" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B595" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C595" s="27">
         <v>483878</v>
@@ -19066,7 +19102,7 @@
     </row>
     <row r="596" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B596" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C596" s="27">
         <v>484014</v>
@@ -19407,10 +19443,10 @@
     </row>
     <row r="607" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A607" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B607" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C607" s="27">
         <v>514453</v>
@@ -19426,7 +19462,7 @@
     </row>
     <row r="608" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B608" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C608" s="27">
         <v>516536</v>
@@ -19767,10 +19803,10 @@
     </row>
     <row r="619" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A619" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B619" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C619" s="27">
         <v>94737</v>
@@ -19786,7 +19822,7 @@
     </row>
     <row r="620" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B620" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C620" s="27">
         <v>94844</v>
@@ -20127,10 +20163,10 @@
     </row>
     <row r="631" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A631" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B631" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C631" s="27">
         <v>63463</v>
@@ -20146,7 +20182,7 @@
     </row>
     <row r="632" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B632" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C632" s="27">
         <v>63386</v>
@@ -20487,10 +20523,10 @@
     </row>
     <row r="643" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A643" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B643" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C643" s="27">
         <v>13786</v>
@@ -20506,7 +20542,7 @@
     </row>
     <row r="644" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B644" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C644" s="27">
         <v>13821</v>
@@ -20847,10 +20883,10 @@
     </row>
     <row r="655" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A655" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B655" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C655" s="27">
         <v>442179</v>
@@ -20866,7 +20902,7 @@
     </row>
     <row r="656" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B656" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C656" s="27">
         <v>442343</v>
@@ -21207,10 +21243,10 @@
     </row>
     <row r="667" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A667" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B667" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C667" s="27">
         <v>55365</v>
@@ -21226,7 +21262,7 @@
     </row>
     <row r="668" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B668" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C668" s="27">
         <v>55313</v>
@@ -21579,10 +21615,10 @@
     </row>
     <row r="680" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A680" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B680" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C680" s="27">
         <v>823318</v>
@@ -21598,7 +21634,7 @@
     </row>
     <row r="681" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B681" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C681" s="27">
         <v>825009</v>
@@ -21939,10 +21975,10 @@
     </row>
     <row r="692" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A692" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B692" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C692" s="27">
         <v>200849</v>
@@ -21958,7 +21994,7 @@
     </row>
     <row r="693" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B693" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C693" s="27">
         <v>202503</v>
@@ -22299,10 +22335,10 @@
     </row>
     <row r="704" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A704" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B704" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C704" s="27">
         <v>72155</v>
@@ -22318,7 +22354,7 @@
     </row>
     <row r="705" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B705" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C705" s="27">
         <v>72408</v>
@@ -22659,7 +22695,7 @@
     </row>
     <row r="716" spans="1:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A716" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B716" s="14"/>
       <c r="C716" s="13"/>
@@ -22668,7 +22704,7 @@
     </row>
     <row r="717" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A717" s="67" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B717" s="14"/>
       <c r="C717" s="13"/>
@@ -22677,7 +22713,7 @@
     </row>
     <row r="718" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A718" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B718" s="15"/>
       <c r="C718" s="13"/>

</xml_diff>